<commit_message>
Big batch of changes
</commit_message>
<xml_diff>
--- a/tests/testthat/macierze_analiz.xlsx
+++ b/tests/testthat/macierze_analiz.xlsx
@@ -222,55 +222,58 @@
     <t>prefix1:</t>
   </si>
   <si>
-    <t>flag_gr_after_indep: 1
+    <t>prefix2: [Zmienne demograficzne, {1, Data urodzenia}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Zmienne demograficzne, {1, Płeć}]</t>
+  </si>
+  <si>
+    <t>prefix2: Śmierć</t>
+  </si>
+  <si>
+    <t>prefix2: [Zmienne demograficzne, {2, Masa ciała}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Zmienne demograficzne, {2, Masa ciała}, Dymorfizm masy ciała]</t>
+  </si>
+  <si>
+    <t>prefix2: [Zmienne demograficzne, {3, Skala Apgar i miesiące ciąży}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Zmienne demograficzne, {4,Typ porodu}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Komplikacje okołoporodowe, {1, "&lt;depvar&gt;"}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Komplikacje okołoporodowe, {2, "&lt;depvar&gt;"}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Komplikacje okołoporodowe, {3, "&lt;depvar&gt;"}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Komplikacje okołoporodowe, {4, "&lt;depvar&gt;"}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Komplikacje okołoporodowe, {5, "&lt;depvar&gt;"}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Komplikacje okołoporodowe, {6, "&lt;depvar&gt;"}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Komplikacje okołoporodowe, {7, "&lt;depvar&gt;"}]</t>
+  </si>
+  <si>
+    <t>prefix2: [Zmienne demograficzne, {4,Wiek matki}]</t>
+  </si>
+  <si>
+    <t>table_group_first: 0
 prefix2: [20, Reszta analiz]
 prefix1: Analizy
-language: PL</t>
-  </si>
-  <si>
-    <t>prefix2: [Zmienne demograficzne, {1, Data urodzenia}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Zmienne demograficzne, {1, Płeć}]</t>
-  </si>
-  <si>
-    <t>prefix2: Śmierć</t>
-  </si>
-  <si>
-    <t>prefix2: [Zmienne demograficzne, {2, Masa ciała}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Zmienne demograficzne, {2, Masa ciała}, Dymorfizm masy ciała]</t>
-  </si>
-  <si>
-    <t>prefix2: [Zmienne demograficzne, {3, Skala Apgar i miesiące ciąży}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Zmienne demograficzne, {4,Typ porodu}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Komplikacje okołoporodowe, {1, "&lt;depvar&gt;"}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Komplikacje okołoporodowe, {2, "&lt;depvar&gt;"}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Komplikacje okołoporodowe, {3, "&lt;depvar&gt;"}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Komplikacje okołoporodowe, {4, "&lt;depvar&gt;"}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Komplikacje okołoporodowe, {5, "&lt;depvar&gt;"}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Komplikacje okołoporodowe, {6, "&lt;depvar&gt;"}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Komplikacje okołoporodowe, {7, "&lt;depvar&gt;"}]</t>
-  </si>
-  <si>
-    <t>prefix2: [Zmienne demograficzne, {4,Wiek matki}]</t>
+language: PL
+period_unit: year
+period_value: 1
+include_smoothed_periodogram: 1</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>252405</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -473,7 +476,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>77805</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -805,7 +808,7 @@
   <dimension ref="A1:AF27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -830,7 +833,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="57">
+    <row r="2" spans="1:32" ht="114">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -838,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>51</v>
@@ -971,7 +974,7 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
@@ -1054,7 +1057,7 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -1144,7 +1147,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1225,7 +1228,7 @@
     </row>
     <row r="9" spans="1:32">
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1306,7 +1309,7 @@
     </row>
     <row r="10" spans="1:32">
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1390,7 +1393,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>37</v>
@@ -1474,7 +1477,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>37</v>
@@ -1558,7 +1561,7 @@
     </row>
     <row r="13" spans="1:32">
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1642,7 +1645,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1687,7 +1690,7 @@
     </row>
     <row r="15" spans="1:32">
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1771,7 +1774,7 @@
     </row>
     <row r="16" spans="1:32">
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -1851,7 +1854,7 @@
     </row>
     <row r="17" spans="3:32">
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
         <v>40</v>
@@ -1910,7 +1913,7 @@
     </row>
     <row r="18" spans="3:32">
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1994,7 +1997,7 @@
     </row>
     <row r="19" spans="3:32">
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
@@ -2080,7 +2083,7 @@
     </row>
     <row r="20" spans="3:32">
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
@@ -2157,7 +2160,7 @@
     </row>
     <row r="21" spans="3:32">
       <c r="C21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>43</v>
@@ -2234,7 +2237,7 @@
     </row>
     <row r="22" spans="3:32">
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
         <v>44</v>
@@ -2311,7 +2314,7 @@
     </row>
     <row r="23" spans="3:32">
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
         <v>45</v>
@@ -2397,7 +2400,7 @@
     </row>
     <row r="24" spans="3:32">
       <c r="C24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
@@ -2557,7 +2560,7 @@
     </row>
     <row r="26" spans="3:32">
       <c r="C26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>

</xml_diff>